<commit_message>
[feature] Modelos e fabricantes adicionados aos ativos
</commit_message>
<xml_diff>
--- a/completassov2.xlsx
+++ b/completassov2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDriveFalse\1 - KevDev\2 - Estudos\Testes de codigo\GLPI scripts\Input de informações e criação de coisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24DCF29-3126-45C4-A397-900B560AC494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F110489A-1166-4B6E-AC23-6344C5101112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GLPI Input" sheetId="1" r:id="rId1"/>
@@ -226,9 +226,6 @@
     <t>Tipo de Linha</t>
   </si>
   <si>
-    <t>Tipo de Telefone</t>
-  </si>
-  <si>
     <t>Data Inicial linha</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>Checkin Notebook</t>
   </si>
   <si>
-    <t>Fabricante telefone</t>
-  </si>
-  <si>
     <t>Armazenamento Notebook</t>
   </si>
   <si>
@@ -284,6 +278,12 @@
   </si>
   <si>
     <t>Contrato Linha</t>
+  </si>
+  <si>
+    <t>Marca do Celular</t>
+  </si>
+  <si>
+    <t>Tipo de Celular</t>
   </si>
 </sst>
 </file>
@@ -640,7 +640,7 @@
   <dimension ref="A1:AG11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,10 +655,13 @@
     <col min="10" max="11" width="13.140625" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.140625" customWidth="1"/>
-    <col min="14" max="14" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="22" width="16.140625" customWidth="1"/>
+    <col min="14" max="14" width="16.140625" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="16.140625" customWidth="1"/>
     <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="20" customWidth="1"/>
     <col min="25" max="25" width="26.28515625" bestFit="1" customWidth="1"/>
@@ -698,49 +701,49 @@
         <v>66</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>67</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="X1" s="1" t="s">
         <v>7</v>
@@ -749,28 +752,28 @@
         <v>8</v>
       </c>
       <c r="Z1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB1" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="AA1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="AC1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AD1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.25">
@@ -789,10 +792,10 @@
       <c r="G2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>14</v>
       </c>
       <c r="W2" t="s">
@@ -841,10 +844,10 @@
       <c r="G4" t="s">
         <v>26</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>27</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>28</v>
       </c>
       <c r="W4" t="s">
@@ -887,10 +890,10 @@
       <c r="G6" t="s">
         <v>37</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>38</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>39</v>
       </c>
     </row>
@@ -947,10 +950,10 @@
       <c r="G9" t="s">
         <v>50</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>51</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -993,10 +996,10 @@
       <c r="G11" t="s">
         <v>60</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>61</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[feature] Users, lines and notebooks aditional infos added
</commit_message>
<xml_diff>
--- a/completassov2.xlsx
+++ b/completassov2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OneDriveFalse\1 - KevDev\2 - Estudos\Testes de codigo\GLPI scripts\Input de informações e criação de coisas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F110489A-1166-4B6E-AC23-6344C5101112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E934DE2B-7105-4D16-9C2A-CF234ADE3645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30612" yWindow="1968" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GLPI Input" sheetId="1" r:id="rId1"/>
@@ -639,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,11 +664,11 @@
     <col min="20" max="22" width="16.140625" customWidth="1"/>
     <col min="23" max="23" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="20" customWidth="1"/>
-    <col min="25" max="25" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="14" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="23.140625" bestFit="1" customWidth="1"/>
@@ -682,7 +682,7 @@
       <c r="B1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>65</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -697,7 +697,7 @@
       <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>66</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -749,19 +749,19 @@
         <v>7</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="AD1" s="2" t="s">
         <v>78</v>
@@ -780,6 +780,9 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
+      <c r="C2">
+        <v>35686234657</v>
+      </c>
       <c r="D2" t="s">
         <v>63</v>
       </c>
@@ -804,7 +807,7 @@
       <c r="X2" t="s">
         <v>15</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -812,6 +815,9 @@
       <c r="A3" t="s">
         <v>18</v>
       </c>
+      <c r="C3">
+        <v>35686234658</v>
+      </c>
       <c r="D3" t="s">
         <v>63</v>
       </c>
@@ -824,7 +830,7 @@
       <c r="X3" t="s">
         <v>20</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -832,6 +838,9 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
+      <c r="C4">
+        <v>35686234659</v>
+      </c>
       <c r="D4" t="s">
         <v>63</v>
       </c>
@@ -856,7 +865,7 @@
       <c r="X4" t="s">
         <v>29</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -864,6 +873,9 @@
       <c r="A5" t="s">
         <v>32</v>
       </c>
+      <c r="C5">
+        <v>35686234660</v>
+      </c>
       <c r="D5" t="s">
         <v>63</v>
       </c>
@@ -878,6 +890,9 @@
       <c r="A6" t="s">
         <v>34</v>
       </c>
+      <c r="C6">
+        <v>35686234661</v>
+      </c>
       <c r="D6" t="s">
         <v>63</v>
       </c>
@@ -901,6 +916,9 @@
       <c r="A7" t="s">
         <v>40</v>
       </c>
+      <c r="C7">
+        <v>35686234662</v>
+      </c>
       <c r="D7" t="s">
         <v>63</v>
       </c>
@@ -910,7 +928,7 @@
       <c r="X7" t="s">
         <v>41</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="Z7" t="s">
         <v>42</v>
       </c>
     </row>
@@ -918,6 +936,9 @@
       <c r="A8" t="s">
         <v>43</v>
       </c>
+      <c r="C8">
+        <v>35686234663</v>
+      </c>
       <c r="D8" t="s">
         <v>63</v>
       </c>
@@ -933,7 +954,7 @@
       <c r="X8" t="s">
         <v>45</v>
       </c>
-      <c r="Y8" t="s">
+      <c r="Z8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -941,6 +962,9 @@
       <c r="A9" t="s">
         <v>48</v>
       </c>
+      <c r="C9">
+        <v>35686234664</v>
+      </c>
       <c r="D9" t="s">
         <v>63</v>
       </c>
@@ -961,6 +985,9 @@
       <c r="A10" t="s">
         <v>53</v>
       </c>
+      <c r="C10">
+        <v>35686234665</v>
+      </c>
       <c r="D10" t="s">
         <v>63</v>
       </c>
@@ -976,13 +1003,16 @@
       <c r="X10" t="s">
         <v>55</v>
       </c>
-      <c r="Y10" t="s">
+      <c r="Z10" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
+      </c>
+      <c r="C11">
+        <v>35686234666</v>
       </c>
       <c r="D11" t="s">
         <v>63</v>

</xml_diff>